<commit_message>
Xóa trình độ Cao đẳng
</commit_message>
<xml_diff>
--- a/dang_ky.xlsx
+++ b/dang_ky.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2584,6 +2584,116 @@
         </is>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Nguyễn Thị Phương Anh</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Bác sĩ</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Khoa Liên chuyên khoa</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Có</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>0363558688</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Phuonganhhom@gmail.com</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>2025-02-24 08:25:11</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>12/07/1993</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>Điều dưỡng</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>Cao đẳng</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Phạm Thị Thu</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Bác sĩ</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Khoa Liên chuyên khoa</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Có</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>0983564922</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>bsthubvdonganh@gmail.com</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>2025-02-24 08:26:08</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>19/11/1983</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>Bác sỹ</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>ThS</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>